<commit_message>
update bulk list upload
</commit_message>
<xml_diff>
--- a/boo_mep/public/plantillas/PlantillaEstudiantes.xlsx
+++ b/boo_mep/public/plantillas/PlantillaEstudiantes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\OneDrive\Documentos\Proyectos 2024\Proyecto MEP\BOO_MEP\boo_mep\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516E5E26-9875-4214-8AD9-D2B9BD60136D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BFFD03-B4CA-45C3-A067-519B8C91C54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26040" yWindow="2505" windowWidth="24300" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Primer Nombre</t>
-  </si>
-  <si>
     <t>Primer Apellido</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>Identificacion</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,16 +382,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>